<commit_message>
Add a citation for Movebank study 9165543
</commit_message>
<xml_diff>
--- a/Table S6_movebank_studies.xlsx
+++ b/Table S6_movebank_studies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qiqiy/Documents/P2_WAI/manuscript/Supplimentary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qiqiy/Documents/P2_WAI/manuscript/HPAI_Bird_world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103B534A-42B5-1D47-9BB9-0B73F73C9C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F64232-5416-D044-B057-B721BA2F6538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12440" windowHeight="16800" xr2:uid="{7F6C678B-15DD-314D-A247-D7842A8B8643}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16240" xr2:uid="{7F6C678B-15DD-314D-A247-D7842A8B8643}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,10 +106,6 @@
     <t>1. Arlt D, Olsson P, Fox JW, Low M, Pärt T (2015) Prolonged stopover duration characterises migration strategy and constraints of a long-distant migrant songbird. Animal Migration 2(1): 47–62. doi:10.1515/ami-2015-0002; 2. Arlt D, Olsson P, Fox JW, Low M, Pärt T. 2015. Data from: Prolonged stopover duration characterises migration strategy and constraints of a long-distant migrant songbird. Movebank Data Repository. https://www.doi.org/10.5441/001/1.nn55rh75</t>
   </si>
   <si>
-    <t>1.Tucker, M. A. et al. Large birds travel farther in homogeneous environments. Global Ecol Biogeogr 28, 576–587 (2019).
-2.Efrat, R., Harel, R., Alexandrou, O., Catsadorakis, G. &amp; Nathan, R. Seasonal differences in energy expenditure, flight characteristics and spatial utilization of Dalmatian Pelicans Pelecanus crispus in Greece. Ibis 161, 415–427 (2019).</t>
-  </si>
-  <si>
     <t>1. Movebank Data Repository with DOI 10.5441/001/1.7856r086; 2. Lamb JS, Satgé YG, Jodice PGR (2017) Influence of density-dependent competition on foraging and migratory behavior of a subtropical colonial seabird. Ecology and Evolution 7(16): 6469–6481. doi: 10.1002/ece3.3216</t>
   </si>
   <si>
@@ -519,6 +515,10 @@
   </si>
   <si>
     <t>1. Petersen MR, Douglas DC. 2016. Data from: At-sea distribution of spectacled eiders: a 120-year-old mystery resolved. Movebank Data Repository. https://doi.org/10.5441/001/1.kq7t609j 2. Sexson MG, Petersen MR, Breed GA, Powell AN. 2016. Shifts in the distribution of molting spectacled eiders (Somateria fischeri) indicate ecosystem change in the Arctic. The Condor. 118(3):463-476. https://doi.org/10.1650/CONDOR-15-139.1    3. Petersen MR, Douglas DC. 2004. Winter ecology of spectacled eiders: environmental characteristics and population change. The Condor. 106(1):79-94. http://www.jstor.org/stable/1370518    4.Petersen MR, Grand JB, Dau CP. 2000. Spectacled eider (Somateria fischeri). The Birds of North America online (Rodewald PG, Ed), Cornell Lab of Ornithology, Ithaca, NY. doi:10.2173/bna.547. https://birdsna.org/Species-Account/bna/species/speeid   5. Petersen MR, Larned WW, Douglas DC. 1999. At-sea distribution of spectacled eiders: a 120-year-old mystery resolved. The Auk. 116(4):1009–1020. https://doi.org/10.2307/4089681   6. Petersen MR, Douglas DC, Mulcahy DM. 1995. Use of implanted satellite transmitters to locate spectacled eiders at-sea. The Condor. 97(1):276–278. http://www.jstor.org/stable/1369006</t>
+  </si>
+  <si>
+    <t>1.Tucker, M. A. et al. Large birds travel farther in homogeneous environments. Global Ecol Biogeogr 28, 576–587 (2019).
+2.Efrat, R., Harel, R., Alexandrou, O., Catsadorakis, G. &amp; Nathan, R. Seasonal differences in energy expenditure, flight characteristics and spatial utilization of Dalmatian Pelicans Pelecanus crispus in Greece. Ibis 161, 415–427 (2019). 3. Georgopoulou, E., Alexandrou, O., Manolopoulos, A., Xirouchakis, S. &amp; Catsadorakis, G. (2023) Home range of the Dalmatian pelican in south‑east Europe. European Journal of Wildlife Research 69:41. https://doi.org/10.1007/s10344-023-01667-1</t>
   </si>
 </sst>
 </file>
@@ -577,7 +577,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -865,7 +865,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45720B17-671F-B445-BCAD-CEB390ACD3FD}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -889,22 +889,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -912,13 +912,13 @@
         <v>8927992</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -932,13 +932,13 @@
         <v>3109235</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
@@ -952,13 +952,13 @@
         <v>446579</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>3</v>
@@ -972,13 +972,13 @@
         <v>11017705</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
@@ -992,13 +992,13 @@
         <v>163020445</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
@@ -1012,13 +1012,13 @@
         <v>133992043</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
@@ -1032,16 +1032,16 @@
         <v>49535504</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F8">
         <v>2021</v>
@@ -1052,13 +1052,13 @@
         <v>446487</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>7</v>
@@ -1072,13 +1072,13 @@
         <v>8849813</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
@@ -1092,13 +1092,13 @@
         <v>78970444</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
@@ -1112,13 +1112,13 @@
         <v>446575</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>8</v>
@@ -1132,13 +1132,13 @@
         <v>1495582</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>9</v>
@@ -1152,13 +1152,13 @@
         <v>1518377</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>9</v>
@@ -1172,16 +1172,16 @@
         <v>29799425</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F15">
         <v>2021</v>
@@ -1192,13 +1192,13 @@
         <v>2231619</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>10</v>
@@ -1212,10 +1212,10 @@
         <v>125221</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>1</v>
@@ -1229,13 +1229,13 @@
         <v>34551859</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>11</v>
@@ -1249,13 +1249,13 @@
         <v>164144882</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>12</v>
@@ -1269,13 +1269,13 @@
         <v>204253</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>13</v>
@@ -1289,13 +1289,13 @@
         <v>2354282</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>14</v>
@@ -1309,13 +1309,13 @@
         <v>11468393</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>15</v>
@@ -1329,13 +1329,13 @@
         <v>332044860</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>16</v>
@@ -1349,16 +1349,16 @@
         <v>74496970</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F24">
         <v>2021</v>
@@ -1369,13 +1369,13 @@
         <v>92261778</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>1</v>
@@ -1389,13 +1389,13 @@
         <v>178797918</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>17</v>
@@ -1409,16 +1409,16 @@
         <v>16615296</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F27">
         <v>2021</v>
@@ -1429,13 +1429,13 @@
         <v>6770990</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>1</v>
@@ -1449,13 +1449,13 @@
         <v>45989874</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>1</v>
@@ -1469,16 +1469,16 @@
         <v>2919708</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F30">
         <v>2021</v>
@@ -1489,13 +1489,13 @@
         <v>129159787</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>18</v>
@@ -1509,13 +1509,13 @@
         <v>10204361</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>1</v>
@@ -1529,13 +1529,13 @@
         <v>20873986</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>1</v>
@@ -1549,16 +1549,16 @@
         <v>2988333</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F34">
         <v>2021</v>
@@ -1569,13 +1569,13 @@
         <v>312267867</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>1</v>
@@ -1589,13 +1589,13 @@
         <v>66480086</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>19</v>
@@ -1609,16 +1609,16 @@
         <v>305974507</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F37">
         <v>2021</v>
@@ -1629,13 +1629,13 @@
         <v>58672150</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>20</v>
@@ -1644,21 +1644,21 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>9165543</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>21</v>
+        <v>157</v>
       </c>
       <c r="F39">
         <v>2021</v>
@@ -1669,16 +1669,16 @@
         <v>296027617</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F40">
         <v>2021</v>
@@ -1689,16 +1689,16 @@
         <v>24795474</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F41">
         <v>2021</v>
@@ -1709,16 +1709,16 @@
         <v>126313959</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F42">
         <v>2021</v>
@@ -1729,16 +1729,16 @@
         <v>177841261</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F43">
         <v>2021</v>
@@ -1749,16 +1749,16 @@
         <v>152496827</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F44">
         <v>2021</v>
@@ -1769,16 +1769,16 @@
         <v>276604823</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F45">
         <v>2021</v>
@@ -1789,16 +1789,16 @@
         <v>220078181</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F46">
         <v>2021</v>
@@ -1809,16 +1809,16 @@
         <v>121041109</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F47">
         <v>2021</v>
@@ -1829,16 +1829,16 @@
         <v>180290122</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F48">
         <v>2021</v>
@@ -1849,16 +1849,16 @@
         <v>350174730</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C49" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" t="s">
         <v>90</v>
       </c>
-      <c r="D49" t="s">
-        <v>91</v>
-      </c>
       <c r="E49" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F49">
         <v>2021</v>
@@ -1869,16 +1869,16 @@
         <v>132686329</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F50">
         <v>2021</v>
@@ -1889,16 +1889,16 @@
         <v>1685854071</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F51">
         <v>2021</v>
@@ -1906,19 +1906,19 @@
     </row>
     <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" t="s">
         <v>146</v>
       </c>
-      <c r="B52" t="s">
-        <v>148</v>
-      </c>
-      <c r="C52" t="s">
-        <v>147</v>
-      </c>
       <c r="D52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F52">
         <v>2021</v>
@@ -1929,13 +1929,13 @@
         <v>42451582</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C53" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>1</v>
@@ -1949,13 +1949,13 @@
         <v>179241034</v>
       </c>
       <c r="B54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D54" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Add a citation for Movebank study 179241034
</commit_message>
<xml_diff>
--- a/Table S6_movebank_studies.xlsx
+++ b/Table S6_movebank_studies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qiqiy/Documents/P2_WAI/manuscript/HPAI_Bird_world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F64232-5416-D044-B057-B721BA2F6538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823ABF15-B1B5-3546-B821-6B052F21BF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16240" xr2:uid="{7F6C678B-15DD-314D-A247-D7842A8B8643}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="15080" xr2:uid="{7F6C678B-15DD-314D-A247-D7842A8B8643}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="159">
   <si>
     <t>Confirmed citation</t>
   </si>
@@ -519,6 +519,9 @@
   <si>
     <t>1.Tucker, M. A. et al. Large birds travel farther in homogeneous environments. Global Ecol Biogeogr 28, 576–587 (2019).
 2.Efrat, R., Harel, R., Alexandrou, O., Catsadorakis, G. &amp; Nathan, R. Seasonal differences in energy expenditure, flight characteristics and spatial utilization of Dalmatian Pelicans Pelecanus crispus in Greece. Ibis 161, 415–427 (2019). 3. Georgopoulou, E., Alexandrou, O., Manolopoulos, A., Xirouchakis, S. &amp; Catsadorakis, G. (2023) Home range of the Dalmatian pelican in south‑east Europe. European Journal of Wildlife Research 69:41. https://doi.org/10.1007/s10344-023-01667-1</t>
+  </si>
+  <si>
+    <t>1. Scott, Teague K., "Movements of White-Headed and White-Backed Vultures" (2020). Boise State University Theses and Dissertations. 1716.10.18122/td/1716/boisestate 2. Movebank Study name, PI, contact person, year of data retrieval</t>
   </si>
 </sst>
 </file>
@@ -875,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45720B17-671F-B445-BCAD-CEB390ACD3FD}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="F48" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1958,7 +1961,7 @@
         <v>144</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c r="F54">
         <v>2021</v>

</xml_diff>